<commit_message>
Added mathhelp, improved output printing
</commit_message>
<xml_diff>
--- a/Teaching/Marking calculator.xlsx
+++ b/Teaching/Marking calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\OneDrive\Documenten\GitHub\OWFSim\Teaching\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B938BAE-6C7D-4F26-988F-8902E0FEF6A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2917B80F-0631-421D-B7E6-4CD0BE2CB3A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-1230" windowWidth="19440" windowHeight="15000" activeTab="3" xr2:uid="{AFCE41C3-0507-4F3D-8312-A199AC543DA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{AFCE41C3-0507-4F3D-8312-A199AC543DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment 1" sheetId="1" r:id="rId1"/>
@@ -1198,7 +1198,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,14 +1247,14 @@
       </c>
       <c r="B2">
         <f>I6</f>
-        <v>100</v>
+        <v>83.25</v>
       </c>
       <c r="C2">
         <v>4</v>
       </c>
       <c r="D2">
         <f>B2*C2</f>
-        <v>400</v>
+        <v>333</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
@@ -1273,14 +1273,14 @@
         <v>9</v>
       </c>
       <c r="L2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="M2">
         <v>30</v>
       </c>
       <c r="N2">
         <f>L2*M2</f>
-        <v>1500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1289,27 +1289,27 @@
       </c>
       <c r="B3">
         <f>N5</f>
-        <v>67.5</v>
+        <v>52.5</v>
       </c>
       <c r="C3">
         <v>20</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3" si="0">B3*C3</f>
-        <v>1350</v>
+        <v>1050</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
       </c>
       <c r="G3">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="H3">
         <v>25</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I4" si="1">G3*H3</f>
-        <v>2500</v>
+        <v>825</v>
       </c>
       <c r="K3" t="s">
         <v>11</v>
@@ -1350,7 +1350,7 @@
       </c>
       <c r="D5">
         <f>SUM(D2:D3)/C5</f>
-        <v>72.916666666666671</v>
+        <v>57.625</v>
       </c>
       <c r="K5" t="s">
         <v>8</v>
@@ -1361,7 +1361,7 @@
       </c>
       <c r="N5">
         <f>SUM(N2:N3)/M5</f>
-        <v>67.5</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1374,7 +1374,7 @@
       </c>
       <c r="I6">
         <f>SUM(I2:I4)/H6</f>
-        <v>100</v>
+        <v>83.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>